<commit_message>
Python Engineer Lambda Covered
</commit_message>
<xml_diff>
--- a/selenium_automations/Stationery & Office Supplies.xlsx
+++ b/selenium_automations/Stationery & Office Supplies.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moinm\Desktop\Python Practice\Core_Python\Selenium_Automations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{CA649B4F-CB9E-4121-BB80-91933C0AE69C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424FF437-CAD8-4EFC-87E2-86783808199F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stationery &amp; Office Supplies" sheetId="1" r:id="rId1"/>
@@ -6802,7 +6802,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -7289,10 +7289,11 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -7648,35 +7649,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E875"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A461" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A847" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38" customWidth="1"/>
-    <col min="2" max="2" width="168.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="94.85546875" customWidth="1"/>
+    <col min="2" max="2" width="85.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -22540,9 +22542,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>